<commit_message>
Inserindo dados em uma planilha formatada
</commit_message>
<xml_diff>
--- a/Meteora Ecommerce.xlsx
+++ b/Meteora Ecommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gribeirodeal\cursos-alura\curso-excel-domine-editor-planilhas-alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8480AE6-55C1-4CA1-939E-DBEF786EA9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6040D725-5895-4171-93A9-F6F58533A1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,11 @@
     <sheet name="Tabela de Produtos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="23">
   <si>
     <t>Produtos</t>
   </si>
@@ -89,19 +88,30 @@
   <si>
     <t>Meteora</t>
   </si>
+  <si>
+    <t>Qtd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,6 +142,13 @@
       <b/>
       <sz val="14"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -306,53 +323,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -369,6 +407,25 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -476,13 +533,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ACDD8594-C6FB-45AB-BA9E-8F1EB3E3DA5F}" name="Table3" displayName="Table3" ref="A3:D23" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A3:D23" xr:uid="{ACDD8594-C6FB-45AB-BA9E-8F1EB3E3DA5F}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D28492A9-579C-4F05-A742-7ACB40A3E915}" name="Produtos" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1E4438B0-5873-45D7-94C1-2DE7F3D6B1D9}" name="Tamanho" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{10732D68-E106-4E50-A393-271DBF29B5C3}" name="Categoria" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ACDD8594-C6FB-45AB-BA9E-8F1EB3E3DA5F}" name="Table3" displayName="Table3" ref="A3:E23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E23" xr:uid="{ACDD8594-C6FB-45AB-BA9E-8F1EB3E3DA5F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D28492A9-579C-4F05-A742-7ACB40A3E915}" name="Produtos" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1E4438B0-5873-45D7-94C1-2DE7F3D6B1D9}" name="Tamanho" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{10732D68-E106-4E50-A393-271DBF29B5C3}" name="Categoria" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{91F7D37B-465A-4B08-8894-63AF3264D30E}" name="Preço Unitário" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{28FE975C-DEE9-44F0-A8FD-097CAC5CC889}" name="Qtd" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -688,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -698,7 +756,8 @@
     <col min="2" max="2" width="11.54296875" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" customWidth="1"/>
     <col min="4" max="4" width="17.81640625" customWidth="1"/>
-    <col min="5" max="26" width="8" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -708,12 +767,14 @@
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
@@ -725,10 +786,12 @@
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -764,6 +827,9 @@
       <c r="D4" s="16">
         <v>25.9</v>
       </c>
+      <c r="E4" s="18">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -778,6 +844,9 @@
       <c r="D5" s="16">
         <v>29.9</v>
       </c>
+      <c r="E5" s="18">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
@@ -792,6 +861,9 @@
       <c r="D6" s="16">
         <v>32.9</v>
       </c>
+      <c r="E6" s="19">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
@@ -806,6 +878,9 @@
       <c r="D7" s="16">
         <v>399.9</v>
       </c>
+      <c r="E7" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -820,6 +895,9 @@
       <c r="D8" s="16">
         <v>249.9</v>
       </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
@@ -834,6 +912,9 @@
       <c r="D9" s="16">
         <v>259.89999999999998</v>
       </c>
+      <c r="E9" s="19">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -848,6 +929,9 @@
       <c r="D10" s="16">
         <v>299.89999999999998</v>
       </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
@@ -862,6 +946,9 @@
       <c r="D11" s="16">
         <v>85.9</v>
       </c>
+      <c r="E11" s="19">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
@@ -876,6 +963,9 @@
       <c r="D12" s="16">
         <v>89.9</v>
       </c>
+      <c r="E12" s="19">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
@@ -890,6 +980,9 @@
       <c r="D13" s="16">
         <v>92.9</v>
       </c>
+      <c r="E13" s="19">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
@@ -904,6 +997,9 @@
       <c r="D14" s="16">
         <v>149.9</v>
       </c>
+      <c r="E14" s="19">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
@@ -918,6 +1014,9 @@
       <c r="D15" s="16">
         <v>65.900000000000006</v>
       </c>
+      <c r="E15" s="19">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
@@ -932,8 +1031,11 @@
       <c r="D16" s="16">
         <v>69.900000000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
@@ -946,8 +1048,11 @@
       <c r="D17" s="16">
         <v>70.900000000000006</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
@@ -960,8 +1065,11 @@
       <c r="D18" s="16">
         <v>199.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
@@ -974,8 +1082,11 @@
       <c r="D19" s="16">
         <v>249.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
@@ -988,8 +1099,11 @@
       <c r="D20" s="16">
         <v>259.89999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1002,8 +1116,11 @@
       <c r="D21" s="16">
         <v>259.89999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
@@ -1016,8 +1133,11 @@
       <c r="D22" s="16">
         <v>39.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
         <v>20</v>
       </c>
@@ -1030,32 +1150,35 @@
       <c r="D23" s="17">
         <v>49.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3970,7 +4093,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3982,7 +4105,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D23"/>
+      <selection activeCell="D4" sqref="D4:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3991,22 +4114,25 @@
     <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="8" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:26" ht="21.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="5.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -4021,7 +4147,9 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4054,8 +4182,11 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="24">
         <v>25.9</v>
+      </c>
+      <c r="E4" s="22">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4068,8 +4199,11 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="24">
         <v>29.9</v>
+      </c>
+      <c r="E5" s="22">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4082,8 +4216,11 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="24">
         <v>32.9</v>
+      </c>
+      <c r="E6" s="22">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4096,8 +4233,11 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="24">
         <v>399.9</v>
+      </c>
+      <c r="E7" s="22">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4110,8 +4250,11 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="24">
         <v>249.9</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4124,8 +4267,11 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="24">
         <v>259.89999999999998</v>
+      </c>
+      <c r="E9" s="22">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4138,8 +4284,11 @@
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="24">
         <v>299.89999999999998</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4152,8 +4301,11 @@
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="24">
         <v>85.9</v>
+      </c>
+      <c r="E11" s="22">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4166,8 +4318,11 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="24">
         <v>89.9</v>
+      </c>
+      <c r="E12" s="22">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4180,8 +4335,11 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="24">
         <v>92.9</v>
+      </c>
+      <c r="E13" s="22">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4194,8 +4352,11 @@
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="24">
         <v>149.9</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4208,8 +4369,11 @@
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="24">
         <v>65.900000000000006</v>
+      </c>
+      <c r="E15" s="22">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4222,11 +4386,14 @@
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="24">
         <v>69.900000000000006</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -4236,11 +4403,14 @@
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="24">
         <v>70.900000000000006</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -4250,11 +4420,14 @@
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="24">
         <v>199.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -4264,11 +4437,14 @@
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="24">
         <v>249.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -4278,11 +4454,14 @@
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="24">
         <v>259.89999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -4292,11 +4471,14 @@
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="24">
         <v>259.89999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -4306,11 +4488,14 @@
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="24">
         <v>39.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -4320,35 +4505,38 @@
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="24">
         <v>49.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -7263,7 +7451,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>